<commit_message>
V 0.3.0, added practice, stremalined some texts.
</commit_message>
<xml_diff>
--- a/data_raw/EHI_dict.xlsx
+++ b/data_raw/EHI_dict.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\EHI\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406D2B28-9609-41D2-BFD0-43BA5C57A2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B089C9-340A-4331-BB18-2D25E9547FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EDT" sheetId="1" r:id="rId1"/>
+    <sheet name="EHI" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="108">
   <si>
     <t>key</t>
   </si>
@@ -63,19 +63,314 @@
     <t>WELCOME</t>
   </si>
   <si>
-    <t>Willkommen zum EmoHI-Test zur Entwicklung der stimmlichen Emotionserkennung von Kindern im Schulalter (Nagels et al., 2020).</t>
-  </si>
-  <si>
-    <t>Willkommen zum EmoHI-Test zur Entwicklung der stimmlichen Emotionserkennung von Kindern im Schulalter (2020).</t>
+    <t>INTRO_TEXT</t>
+  </si>
+  <si>
+    <t>Du wirst 24 verschiedene Klangbeispiele hören, welche sich im emotionalen Ausdruck, in dem sie gesprochen oder gespielt wurden, unterscheiden. Deine Aufgabe ist es auszuwählen, welche der drei vorgegebenen Emotionen deiner Meinung nach am besten zu dem Klangbeispiel passt. Du kannst dir jedes Klangbeispiel zwei Mal anhören. \\ Bitte höre dir die Klangbeispiele immer ganz an, bevor du deine Antwort auswählst. Falls du dir nicht sicher bist, wähle einfach deine beste Vermutung aus. Antworten können sich wiederholen und du kannst mehrmals hintereinander dieselbe Antwortmöglichkeit wählen.</t>
+  </si>
+  <si>
+    <t>Sie werden 24 verschiedene Klangbeispiele hören, welche sich im emotionalen Ausdruck, in dem sie gesprochen oder gespielt wurden, unterscheiden. Ihre Aufgabe ist es auszuwählen, welche der drei vorgegebenen Emotionen Ihrer Meinung nach am besten zu dem Klangbeispiel passt. Sie können sich jedes Klangbeispiel zwei Mal anhören. \\ Bitte hören Sie sich die Klangbeispiele immer ganz an, bevor Sie Ihre Antwort auswählen. Falls Sie sich nicht sicher sind, wählen Sie einfach Ihre beste Vermutung aus. Antworten können sich wiederholen und Sie können mehrmals hintereinander dieselbe Antwortmöglichkeit wählen.</t>
+  </si>
+  <si>
+    <t>You will listen to 24 different sound examples which differ in the emotional expression they transfer. Your task is to decide which of the three predetermined emotions you think fits best. You can hear every sound example twice. \\ Please listen to each sound example in full before making your decision. If you don’t know the answer, give your best guess. Answers may be repeated, so do not worry about making the same selection twice.</t>
+  </si>
+  <si>
+    <t>PROGRESS_TEXT</t>
+  </si>
+  <si>
+    <t>Frage {{num_question}} von {{test_length}}</t>
+  </si>
+  <si>
+    <t>Question {{num_question}} out of {{test_length}}</t>
+  </si>
+  <si>
+    <t>NO_AUDIO</t>
+  </si>
+  <si>
+    <t>Dein Browser unterstützt kein Audio. Dieser Test funktioniert nicht ohne Audio, sorry!</t>
+  </si>
+  <si>
+    <t>Ihr Browser unterstützt kein Audio. Dieser Test funktioniert nicht ohne Audio, sorry!</t>
+  </si>
+  <si>
+    <t>Your browser doesn't support audio. This test won't work without audio, sorry!</t>
+  </si>
+  <si>
+    <t>ITEM_INSTRUCTION</t>
+  </si>
+  <si>
+    <t>Bitte höre dir die folgenden Klangbeispiele an und entscheide, welche Emotion ausgedrückt werden sollte. Klicke dafür eine der jeweils unten stehenden Auswahlmöglichkeiten an.</t>
+  </si>
+  <si>
+    <t>Bitte hören Sie sich die folgenden Klangbeispiele an und entscheiden Sie, welche Emotion ausgedrückt werden sollte. Klicken Sie dafür eine der jeweils unten stehenden Auswahlmöglichkeiten an.</t>
+  </si>
+  <si>
+    <t>Please listen to the following sound examples and decide which emotion is shown. Choose one of the answer options.</t>
+  </si>
+  <si>
+    <t>ERR_NO_SELECTION</t>
+  </si>
+  <si>
+    <t>Bitte eine Option auswählen.</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie eine Option aus.</t>
+  </si>
+  <si>
+    <t>Please select one option.</t>
+  </si>
+  <si>
+    <t>ANGRY</t>
+  </si>
+  <si>
+    <t>wütend</t>
+  </si>
+  <si>
+    <t>angry</t>
+  </si>
+  <si>
+    <t>HAPPY</t>
+  </si>
+  <si>
+    <t>fröhlich</t>
+  </si>
+  <si>
+    <t>happy</t>
+  </si>
+  <si>
+    <t>SAD</t>
+  </si>
+  <si>
+    <t>traurig</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>THANKS</t>
+  </si>
+  <si>
+    <t>Herzlichen Glückwunsch!</t>
+  </si>
+  <si>
+    <t>Congratulations!</t>
+  </si>
+  <si>
+    <t>FEEDBACK</t>
+  </si>
+  <si>
+    <t>Du hast **{{accuracy}} %** der Aufgaben richtig beantwortet.</t>
+  </si>
+  <si>
+    <t>Sie haben **{{accuracy}} %** der Aufgaben richtig beantwortet.</t>
+  </si>
+  <si>
+    <t>You answered **{{accuracy}} %**  of the tasks correctly.</t>
+  </si>
+  <si>
+    <t>ENTER_ID</t>
+  </si>
+  <si>
+    <t>Bitte gib Deine ID ein.</t>
+  </si>
+  <si>
+    <t>Bitte geben Sie Ihre ID ein.</t>
+  </si>
+  <si>
+    <t>Please enter your ID.</t>
+  </si>
+  <si>
+    <t>INVALID_ID</t>
+  </si>
+  <si>
+    <t>Die ID ist leider ungültig. Bitte versuche es noch mal.</t>
+  </si>
+  <si>
+    <t>Die ID ist leider ungültig. Bitte versuchen Sie es noch mal.</t>
+  </si>
+  <si>
+    <t>The ID is invalid. Please try again.</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>Weiter</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+  </si>
+  <si>
+    <t>Du hast den EmoHI-Test für das Erkennen von Emotionen in Sprache erfolgreich beendet.</t>
+  </si>
+  <si>
+    <t>Sie haben den EmoHI-Test für das Erkennen von Emotionen in Sprache erfolgreich beendet.</t>
+  </si>
+  <si>
+    <t>You have completed the EmoHI test for the development of vocal recognition.</t>
+  </si>
+  <si>
+    <t>TESTNAME</t>
+  </si>
+  <si>
+    <t>EmoHI-Test für das Emotionserkennen in Sprache</t>
+  </si>
+  <si>
+    <t>COMPLETED</t>
+  </si>
+  <si>
+    <t>Du hast {{num_correct}} von {{num_question}} Aufgaben richtig beantwortet.</t>
+  </si>
+  <si>
+    <t>Sie haben {{num_correct}} von {{num_question}} Aufgaben richtig beantwortet.</t>
+  </si>
+  <si>
+    <t>You answered {{num_correct}} out of {{num_question}} questions correctly.</t>
+  </si>
+  <si>
+    <t>SCORE_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Dein Testergebnis</t>
+  </si>
+  <si>
+    <t>Ihr Testergebnis</t>
+  </si>
+  <si>
+    <t>Your score</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>Werte</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>GOBACK</t>
+  </si>
+  <si>
+    <t>Gehe zurück</t>
+  </si>
+  <si>
+    <t>Go back</t>
+  </si>
+  <si>
+    <t>VOLUME</t>
+  </si>
+  <si>
+    <t>Stellen Sie nun die Lautstärke ein. Hören Sie sich dazu das Audiobeispiel so oft wie nötig an und stellen Sie sicher, dass Sie den*die Sprecher*in gut verstehen können. Wenn Sie die Lautstärke richtig eingestellt haben, klicken Sie auf „weiter“.</t>
+  </si>
+  <si>
+    <t>Now adjust the volume. Listen to the audio sample as often as necessary and make sure that you can understand the speaker well. When you have set the volume correctly, click "Next".</t>
+  </si>
+  <si>
+    <t>TRANSITION</t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ Klicke auf 'Zurück', um die Anweisungen erneut zu lesen und die Beispiele erneut zu versuchen, oder klicke auf 'Weiter', um zum  Haupttest zu gelangen.</t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ Klicken Sie auf 'Zurück', um die Anweisungen erneut zu lesen und die Beispiele erneut zu versuchen, oder klicken Sie auf 'Weiter', um zum  Haupttest zu gelangen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**{{feedback}}** \\ Press ‘Go back’ to read the instructions and do the practice questions again, or press ‘Continue’ to continue to the main test. </t>
+  </si>
+  <si>
+    <t>MAIN_INTRO</t>
+  </si>
+  <si>
+    <t>Nun geht es mit dem Haupttest los, in dem deine Ergebnisse gespeichert werden. \\ Du bekommst keine Rückmeldung nach den einzelnen Aufgaben. Viel Erfolg!</t>
+  </si>
+  <si>
+    <t>Nun geht es mit dem Haupttest los, in dem Ihre Ergebnisse gespeichert werden. \\ Sie bekommen keine Rückmeldung nach den einzelnen Aufgaben. Viel Erfolg!</t>
+  </si>
+  <si>
+    <t>You are about to start the main test, where your results will be recorded. \\ You won't receive any feedback after individual questions. Good luck!</t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ **Übungsfrage 3** \\ Bitte höre dir das folgende Klangbeispiel an und wähle aus, ob es für dich **wütend**, **fröhlich** oder **traurig** klingt.</t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ **Übungsfrage 2** \\ Bitte höre dir das folgende Klangbeispiel an und wähle aus, ob es für dich **wütend**, **fröhlich** oder **traurig** klingt.</t>
+  </si>
+  <si>
+    <t>Stelle nun die Lautstärke ein. Höre dir dazu das Audiobeispiel so oft wie nötig an und stelle sicher, dass du die Sprecher*in gut verstehen kannst. Wenn du die Lautstärke richtig eingestellt hast, klicke auf „weiter“.</t>
+  </si>
+  <si>
+    <t>**Übungsfrage 1** \\ Bitte hören Sie sich das folgende Klangbeispiel an und wählen Sie aus, ob es für Sie **wütend**, **fröhlich** oder **traurig** klingt.</t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ **Übungsfrage 2** \\ Bitte hören Sie sich das folgende Klangbeispiel an und wählen Sie aus, ob es für Sie **wütend**, **fröhlich** oder **traurig** klingt.</t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ **Übungsfrage 3** \\ Bitte hören Sie sich das folgende Klangbeispiel an und wählen Sie aus, ob es für Sie **wütend**, **fröhlich** oder **traurig** klingt.</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS</t>
+  </si>
+  <si>
+    <t>Du wirst 24 verschiedene Klangbeispiele hören, welche sich im emotionalen Ausdruck, in dem sie gesprochen oder gespielt wurden, unterscheiden. Deine Aufgabe ist es auszuwählen, welche der drei vorgegebenen Emotionen deiner Meinung nach am besten zu dem Klangbeispiel passt. Du kannst dir jedes Klangbeispiel zwei Mal anhören. \\ Bitte höre dir die Klangbeispiele immer ganz an, bevor du deine Antwort auswählst. Falls du dir nicht sicher bist, wähle einfach deine beste Vermutung aus. Antworten können sich wiederholen und du kannst mehrmals hintereinander dieselbe Antwortmöglichkeit wählen.\\ Zunächst kommen **drei Übungsaufgaben**, bevor es mit dem Haupttest losgeht.</t>
+  </si>
+  <si>
+    <t>Sie werden 24 verschiedene Klangbeispiele hören, welche sich im emotionalen Ausdruck, in dem sie gesprochen oder gespielt wurden, unterscheiden. Ihre Aufgabe ist es auszuwählen, welche der drei vorgegebenen Emotionen Ihrer Meinung nach am besten zu dem Klangbeispiel passt. Sie können sich jedes Klangbeispiel zwei Mal anhören. \\ Bitte hören Sie sich die Klangbeispiele immer ganz an, bevor Sie Ihre Antwort auswählen. Falls Sie sich nicht sicher sind, wählen Sie einfach Ihre beste Vermutung aus. Antworten können sich wiederholen und Sie können mehrmals hintereinander dieselbe Antwortmöglichkeit wählen.\\ Zunächst kommen **drei Übungsaufgaben**, bevor es mit dem Haupttest losgeht.</t>
+  </si>
+  <si>
+    <t>You will listen to 24 different sound examples which differ in the emotional expression they transfer. Your task is to decide which of the three predetermined emotions you think fits best. You can hear every sound example twice. \\ Please listen to each sound example in full before making your decision. If you don’t know the answer, give your best guess. Answers may be repeated, so do not worry about making the same selection twice.\\ First, you will get **three practice tasks**, before the main test starts.</t>
+  </si>
+  <si>
+    <t>CORRECT</t>
+  </si>
+  <si>
+    <t>**Richtig!**</t>
+  </si>
+  <si>
+    <t>**Correct!**</t>
+  </si>
+  <si>
+    <t>INCORRECT</t>
+  </si>
+  <si>
+    <t>**Leider falsch.**</t>
+  </si>
+  <si>
+    <t>**Sorry, this was Incorrect.**</t>
+  </si>
+  <si>
+    <t>PRACTICE1</t>
+  </si>
+  <si>
+    <t>PRACTICE2</t>
+  </si>
+  <si>
+    <t>PRACTICE3</t>
+  </si>
+  <si>
+    <t>**Übungsfrage 1** \\ Bitte höre dir das folgende Klangbeispiel an und wähle aus, ob es für dich **wütend**,  **fröhlich** oder **traurig** klingt.</t>
+  </si>
+  <si>
+    <t>**Practice question 1** \\ Please listen to the following sound example and select whether it sounded **angry**, **happy**, or **sad** to you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> **{{feedback}}** \\ **Practice question 2** \\ Please listen to the following sound example and select whether it sounded **angry**, **happy**,  or **sad** to you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> **{{feedback}}** \\ **Practice question 3** \\ Please listen to the following sound example and select whether it sounded **angry**, **happy**, or **sad** to you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmoHI test of vocal emotion recognition </t>
+  </si>
+  <si>
+    <t>Willkommen zum EmoHI-Test zur stimmlichen Emotionserkennung.</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Welcome to the EmoHI test for the development of vocal emotion recognition in school-age children (Nagels et al., 2020).</t>
+      <t>Welcome to the EmoHI test for vocal emotion recognition.</t>
     </r>
     <r>
       <rPr>
@@ -86,267 +381,6 @@
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <t>INTRO_TEXT</t>
-  </si>
-  <si>
-    <t>Du wirst 24 verschiedene Klangbeispiele hören, welche sich im emotionalen Ausdruck, in dem sie gesprochen oder gespielt wurden, unterscheiden. Deine Aufgabe ist es auszuwählen, welche der drei vorgegebenen Emotionen deiner Meinung nach am besten zu dem Klangbeispiel passt. Du kannst dir jedes Klangbeispiel zwei Mal anhören. \\ Bitte höre dir die Klangbeispiele immer ganz an, bevor du deine Antwort auswählst. Falls du dir nicht sicher bist, wähle einfach deine beste Vermutung aus. Antworten können sich wiederholen und du kannst mehrmals hintereinander dieselbe Antwortmöglichkeit wählen.</t>
-  </si>
-  <si>
-    <t>Sie werden 24 verschiedene Klangbeispiele hören, welche sich im emotionalen Ausdruck, in dem sie gesprochen oder gespielt wurden, unterscheiden. Ihre Aufgabe ist es auszuwählen, welche der drei vorgegebenen Emotionen Ihrer Meinung nach am besten zu dem Klangbeispiel passt. Sie können sich jedes Klangbeispiel zwei Mal anhören. \\ Bitte hören Sie sich die Klangbeispiele immer ganz an, bevor Sie Ihre Antwort auswählen. Falls Sie sich nicht sicher sind, wählen Sie einfach Ihre beste Vermutung aus. Antworten können sich wiederholen und Sie können mehrmals hintereinander dieselbe Antwortmöglichkeit wählen.</t>
-  </si>
-  <si>
-    <t>You will listen to 24 different sound examples which differ in the emotional expression they transfer. Your task is to decide which of the three predetermined emotions you think fits best. You can hear every sound example twice. \\ Please listen to each sound example in full before making your decision. If you don’t know the answer, give your best guess. Answers may be repeated, so do not worry about making the same selection twice.</t>
-  </si>
-  <si>
-    <t>PROGRESS_TEXT</t>
-  </si>
-  <si>
-    <t>Frage {{num_question}} von {{test_length}}</t>
-  </si>
-  <si>
-    <t>Question {{num_question}} out of {{test_length}}</t>
-  </si>
-  <si>
-    <t>NO_AUDIO</t>
-  </si>
-  <si>
-    <t>Dein Browser unterstützt kein Audio. Dieser Test funktioniert nicht ohne Audio, sorry!</t>
-  </si>
-  <si>
-    <t>Ihr Browser unterstützt kein Audio. Dieser Test funktioniert nicht ohne Audio, sorry!</t>
-  </si>
-  <si>
-    <t>Your browser doesn't support audio. This test won't work without audio, sorry!</t>
-  </si>
-  <si>
-    <t>ITEM_INSTRUCTION</t>
-  </si>
-  <si>
-    <t>Bitte höre dir die folgenden Klangbeispiele an und entscheide, welche Emotion rübergebracht werden sollte. Klicke dafür eine der jeweils unten stehenden Auswahlmöglichkeiten an.</t>
-  </si>
-  <si>
-    <t>Bitte hören Sie sich die folgenden Klangbeispiele an und entscheiden Sie, welche Emotion rübergebracht werden sollte. Klicken Sie dafür eine der jeweils unten stehenden Auswahlmöglichkeiten an.</t>
-  </si>
-  <si>
-    <t>Please listen to the following sound examples and decide which emotion is shown. Choose one of the answer options.</t>
-  </si>
-  <si>
-    <t>ERR_NO_SELECTION</t>
-  </si>
-  <si>
-    <t>Bitte eine Option auswählen.</t>
-  </si>
-  <si>
-    <t>Bitte wählen Sie eine Option aus.</t>
-  </si>
-  <si>
-    <t>Please select one option.</t>
-  </si>
-  <si>
-    <t>ANGRY</t>
-  </si>
-  <si>
-    <t>wütend</t>
-  </si>
-  <si>
-    <t>angry</t>
-  </si>
-  <si>
-    <t>HAPPY</t>
-  </si>
-  <si>
-    <t>fröhlich</t>
-  </si>
-  <si>
-    <t>happy</t>
-  </si>
-  <si>
-    <t>SAD</t>
-  </si>
-  <si>
-    <t>traurig</t>
-  </si>
-  <si>
-    <t>sad</t>
-  </si>
-  <si>
-    <t>THANKS</t>
-  </si>
-  <si>
-    <t>Herzlichen Glückwunsch!</t>
-  </si>
-  <si>
-    <t>Congratulations!</t>
-  </si>
-  <si>
-    <t>FEEDBACK</t>
-  </si>
-  <si>
-    <t>Du hast **{{accuracy}} %** der Aufgaben richtig beantwortet.</t>
-  </si>
-  <si>
-    <t>Sie haben **{{accuracy}} %** der Aufgaben richtig beantwortet.</t>
-  </si>
-  <si>
-    <t>You answered **{{accuracy}} %**  of the tasks correctly.</t>
-  </si>
-  <si>
-    <t>ENTER_ID</t>
-  </si>
-  <si>
-    <t>Bitte gib Deine ID ein.</t>
-  </si>
-  <si>
-    <t>Bitte geben Sie Ihre ID ein.</t>
-  </si>
-  <si>
-    <t>Please enter your ID.</t>
-  </si>
-  <si>
-    <t>INVALID_ID</t>
-  </si>
-  <si>
-    <t>Die ID ist leider ungültig. Bitte versuche es noch mal.</t>
-  </si>
-  <si>
-    <t>Die ID ist leider ungültig. Bitte versuchen Sie es noch mal.</t>
-  </si>
-  <si>
-    <t>The ID is invalid. Please try again.</t>
-  </si>
-  <si>
-    <t>CONTINUE</t>
-  </si>
-  <si>
-    <t>Weiter</t>
-  </si>
-  <si>
-    <t>Continue</t>
-  </si>
-  <si>
-    <t>SUCCESS</t>
-  </si>
-  <si>
-    <t>Du hast den EmoHI-Test für das Erkennen von Emotionen in Sprache erfolgreich beendet.</t>
-  </si>
-  <si>
-    <t>Sie haben den EmoHI-Test für das Erkennen von Emotionen in Sprache erfolgreich beendet.</t>
-  </si>
-  <si>
-    <t>You have completed the EmoHI test for the development of vocal recognition.</t>
-  </si>
-  <si>
-    <t>TESTNAME</t>
-  </si>
-  <si>
-    <t>EmoHI-Test für das Emotionserkennen in Sprache</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EmoHI test for the development of vocal emotion recognition in school-age children </t>
-  </si>
-  <si>
-    <t>COMPLETED</t>
-  </si>
-  <si>
-    <t>Du hast {{num_correct}} von {{num_question}} Aufgaben richtig beantwortet.</t>
-  </si>
-  <si>
-    <t>Sie haben {{num_correct}} von {{num_question}} Aufgaben richtig beantwortet.</t>
-  </si>
-  <si>
-    <t>You answered {{num_correct}} out of {{num_question}} questions correctly.</t>
-  </si>
-  <si>
-    <t>SCORE_TEMPLATE</t>
-  </si>
-  <si>
-    <t>Dein Testergebnis</t>
-  </si>
-  <si>
-    <t>Ihr Testergebnis</t>
-  </si>
-  <si>
-    <t>Your score</t>
-  </si>
-  <si>
-    <t>VALUE</t>
-  </si>
-  <si>
-    <t>Werte</t>
-  </si>
-  <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>GOBACK</t>
-  </si>
-  <si>
-    <t>Gehe zurück</t>
-  </si>
-  <si>
-    <t>Go back</t>
-  </si>
-  <si>
-    <t>**Übungsfrage 1** \\ Bitte höre dir das folgende Klangbeispiel an und wähle aus, ob es für dich **wütend, fröhlich oder traurig** klingt.</t>
-  </si>
-  <si>
-    <t>**Übungsfrage 1** \\ Bitte hören Sie sich das folgende Klangbeispiel an und wählen Sie aus, ob es für Sie **wütend, fröhlich oder traurig** klingt.</t>
-  </si>
-  <si>
-    <t>**Practice question 1** \\ Please listen to the following sound example and select whether it sounded **angry, happy or sad** to you.</t>
-  </si>
-  <si>
-    <t>**{{feedback}}** \\ **Übungsfrage 2** \\ Bitte höre dir das folgende Klangbeispiel an und wähle aus, ob es für dich **wütend, fröhlich oder traurig** klingt.</t>
-  </si>
-  <si>
-    <t>**{{feedback}}** \\ **Übungsfrage 2** \\ Bitte hören Sie sich das folgende Klangbeispiel an und wählen Sie aus, ob es für Sie **wütend, fröhlich oder traurig** klingt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> **{{feedback}}** \\ **Practice question 2** \\ Please listen to the following sound example and select whether it sounded **angry, happy or sad** to you.</t>
-  </si>
-  <si>
-    <t>**{{feedback}}** \\ **Übungsfrage 3** \\ Bitte höre dir das folgende Klangbeispiel an und wähle aus, ob es für dich **wütend, fröhlich oder traurig** klingt.</t>
-  </si>
-  <si>
-    <t>**{{feedback}}** \\ **Übungsfrage 3** \\ Bitte hören Sie sich das folgende Klangbeispiel an und wählen Sie aus, ob es für Sie **wütend, fröhlich oder traurig** klingt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> **{{feedback}}** \\ **Practice question 3** \\ Please listen to the following sound example and select whether it sounded **angry, happy or sad** to you.</t>
-  </si>
-  <si>
-    <t>TRANSITION</t>
-  </si>
-  <si>
-    <t>**{{feedback}}** \\ Klicke auf 'Zurück', um die Anweisungen erneut zu lesen und die Beispiele erneut zu versuchen, oder klicke auf 'Weiter', um zum  Haupttest zu gelangen.</t>
-  </si>
-  <si>
-    <t>**{{feedback}}** \\ Klicken Sie auf 'Zurück', um die Anweisungen erneut zu lesen und die Beispiele erneut zu versuchen, oder klicken Sie auf 'Weiter', um zum  Haupttest zu gelangen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**{{feedback}}** \\ Press ‘Go back’ to read the instructions and do the practice questions again, or press ‘Continue’ to continue to the main test. </t>
-  </si>
-  <si>
-    <t>MAIN_INTRO</t>
-  </si>
-  <si>
-    <t>Nun geht es mit dem Haupttest los, in dem deine Ergebnisse gespeichert werden. \\ Du bekommst keine Rückmeldung nach den einzelnen Aufgaben. Viel Erfolg!</t>
-  </si>
-  <si>
-    <t>Nun geht es mit dem Haupttest los, in dem Ihre Ergebnisse gespeichert werden. \\ Sie bekommen keine Rückmeldung nach den einzelnen Aufgaben. Viel Erfolg!</t>
-  </si>
-  <si>
-    <t>You are about to start the main test, where your results will be recorded. \\ You won't receive any feedback after individual questions. Good luck!</t>
-  </si>
-  <si>
-    <t>PRACTICE2</t>
-  </si>
-  <si>
-    <t>PRACTICE1</t>
-  </si>
-  <si>
-    <t>PRACTICE3</t>
   </si>
 </sst>
 </file>
@@ -390,7 +424,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -420,19 +454,6 @@
       <right style="thin">
         <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -451,10 +472,14 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1616,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1628,11 +1653,10 @@
     <col min="2" max="2" width="67.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="66.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="55" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1">
+    <row r="1" spans="1:4" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1645,382 +1669,454 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" ht="54.95" customHeight="1">
+    </row>
+    <row r="2" spans="1:4" ht="54.95" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="104.45" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" ht="104.45" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="26.45" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" ht="26.45" customHeight="1">
-      <c r="A5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="39.6" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" ht="39.6" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="7" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="C8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="C15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="26.45" customHeight="1">
+      <c r="A16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" ht="26.45" customHeight="1">
-      <c r="A16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="3" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="26.45" customHeight="1">
+      <c r="A17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="C17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="26.45" customHeight="1">
+      <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="26.45" customHeight="1">
-      <c r="A17" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" ht="26.45" customHeight="1">
-      <c r="A18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="3" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A20" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="3" t="s">
+    </row>
+    <row r="22" spans="1:4" ht="39.6" customHeight="1">
+      <c r="A22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A21" s="2" t="s">
+      <c r="B22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="3" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="26.45" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="39.6" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="39.6" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="39.6" customHeight="1">
+      <c r="A26" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" ht="26.45" customHeight="1">
-      <c r="A22" s="2" t="s">
+      <c r="B26" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="26.45" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="104.45" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1">
+      <c r="A32" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" ht="39.6" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" ht="39.6" customHeight="1">
-      <c r="A24" s="2" t="s">
+      <c r="C32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" ht="39.6" customHeight="1">
-      <c r="A25" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:5" ht="26.45" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="6"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1">
+      <c r="A33" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>